<commit_message>
Add AutoReceiptActivity and its unit test.
</commit_message>
<xml_diff>
--- a/tests/CcintOcrBasicTests/Tests_Data/config/recognizer_config.xlsx
+++ b/tests/CcintOcrBasicTests/Tests_Data/config/recognizer_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenlooplee\Documents\GitHub\CcintOcrActivitiesPack\tests\CcintOcrBasicTests\Tests_Data\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54505FFF-D84C-4CF6-A4C4-3B1C168E275B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38389BE4-F952-4DB0-AE32-ED1F4022518E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18436" windowHeight="11160" xr2:uid="{D6D768DA-5964-4C9E-A98A-0598DDF1AEA9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>AppKey</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>https://ocr-api.ccint.com/cci_ai/service/v1/id_card</t>
+  </si>
+  <si>
+    <t>auto_receipt</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/general_receipt_recog</t>
   </si>
 </sst>
 </file>
@@ -432,16 +438,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41493430-721B-460C-97F1-874FC5931AF2}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.06640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.73046875" bestFit="1" customWidth="1"/>
   </cols>
@@ -493,12 +499,21 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CFF59CB1-5500-4F10-A705-B9374BEF4C9F}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{E56C7ECF-6286-4ABE-B959-11D360773DEB}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{AEB2A04B-2B43-432E-BD45-CDC21EB05396}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{E5C8037E-8AC0-4156-B2B6-8CB87DEB7C4F}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{C1BA6A99-37F0-4BF9-994D-622006E2BEC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update recognizer_config.xlsx for APIs supported by Ccint.
</commit_message>
<xml_diff>
--- a/tests/CcintOcrBasicTests/Tests_Data/config/recognizer_config.xlsx
+++ b/tests/CcintOcrBasicTests/Tests_Data/config/recognizer_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenlooplee\Documents\GitHub\CcintOcrActivitiesPack\tests\CcintOcrBasicTests\Tests_Data\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38389BE4-F952-4DB0-AE32-ED1F4022518E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5CCA4F-1DF5-4025-A129-34DEF77CEEA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18436" windowHeight="11160" xr2:uid="{D6D768DA-5964-4C9E-A98A-0598DDF1AEA9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>AppKey</t>
   </si>
@@ -75,6 +75,48 @@
   </si>
   <si>
     <t>https://ocr-api.ccint.com/cci_ai/service/v1/general_receipt_recog</t>
+  </si>
+  <si>
+    <t>taxi_receipt</t>
+  </si>
+  <si>
+    <t>train_ticket</t>
+  </si>
+  <si>
+    <t>household_register</t>
+  </si>
+  <si>
+    <t>passport</t>
+  </si>
+  <si>
+    <t>driver_license</t>
+  </si>
+  <si>
+    <t>vehicle_license</t>
+  </si>
+  <si>
+    <t>vehicle_certificate</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/taxi_invoice</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/train_ticket</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/household_register</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/passport</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/driver_license</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/vehicle_license</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/vehicle_inspection_certificate</t>
   </si>
 </sst>
 </file>
@@ -438,16 +480,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41493430-721B-460C-97F1-874FC5931AF2}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.73046875" bestFit="1" customWidth="1"/>
   </cols>
@@ -468,52 +510,115 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{CFF59CB1-5500-4F10-A705-B9374BEF4C9F}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{E56C7ECF-6286-4ABE-B959-11D360773DEB}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{AEB2A04B-2B43-432E-BD45-CDC21EB05396}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{E5C8037E-8AC0-4156-B2B6-8CB87DEB7C4F}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{C1BA6A99-37F0-4BF9-994D-622006E2BEC0}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CFF59CB1-5500-4F10-A705-B9374BEF4C9F}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{E56C7ECF-6286-4ABE-B959-11D360773DEB}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{AEB2A04B-2B43-432E-BD45-CDC21EB05396}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{E5C8037E-8AC0-4156-B2B6-8CB87DEB7C4F}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{C1BA6A99-37F0-4BF9-994D-622006E2BEC0}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{6AF3F50C-14D8-4B53-90D0-A1C7FC731270}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{8FBD5B7F-9D45-483D-A5D4-1C0EFEA2C2D5}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{6A54A24A-9C85-4978-BB42-294BB76DEEB2}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{7A212157-0561-4336-B6C6-DAE2CBAF1F7A}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{08E97965-7030-445B-BAF5-A67AB37AF8C3}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{04AA563B-6CF4-44DE-AE3B-11C19452B14F}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{1B2548A1-8719-48FB-9AD3-357F6395DBB9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>